<commit_message>
Modified the documentation, fixed grid get agent bugs.
</commit_message>
<xml_diff>
--- a/examples/Covid/data/excel_source/scenarios.xlsx
+++ b/examples/Covid/data/excel_source/scenarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Dropbox\ABM4ALL\Melodie\examples\Covid\data\excel_source\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12957\Documents\Developing\Python\melodie\examples\Covid\data\excel_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6867EB93-DC8C-483A-8221-7338B714979A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30915" windowHeight="7830"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30915" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exo_ScenarioPara" sheetId="1" r:id="rId1"/>
@@ -48,11 +49,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -79,7 +86,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,14 +363,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -374,7 +381,7 @@
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -400,7 +407,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>0</v>
       </c>
@@ -408,7 +415,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1000</v>
+        <v>300</v>
       </c>
       <c r="D2">
         <v>1000</v>
@@ -427,6 +434,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>